<commit_message>
PHR output - updates to PHS Composition profile to make invariant expressions relative, require section.entry.reference, fix values of CodeableCConcept elements by using pattern and update copyright year & attributions and impplementation guidance; closes #70 & closes #66
</commit_message>
<xml_diff>
--- a/output/PersonalHealthRecords/composition-phs-1.xlsx
+++ b/output/PersonalHealthRecords/composition-phs-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$100</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3063" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="454">
   <si>
     <t>Path</t>
   </si>
@@ -1120,7 +1120,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-02:The section shall at least have one entry or an empty reason, but not both {Composition.section.where($this.entry.empty() and $this.emptyReason.empty()).empty()}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-02:The section shall at least have one entry or an empty reason, but not both {entry.exists() xor emptyReason.exists()}</t>
   </si>
   <si>
     <t>./outboundRelationship[typeCode="COMP" and isNormalActRelationship()]/target[moodCode="EVN" and classCode="DOCSECT" and isNormalAct]</t>
@@ -1353,6 +1353,66 @@
     <t>Allergies and/or intolerances</t>
   </si>
   <si>
+    <t>Composition.section.entry.id</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.extension</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.reference</t>
+  </si>
+  <si>
+    <t>Literal reference, Relative, internal or absolute URL</t>
+  </si>
+  <si>
+    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
+  </si>
+  <si>
+    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
+  </si>
+  <si>
+    <t>Reference.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref-1
+</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.identifier</t>
+  </si>
+  <si>
+    <t>Logical reference, when literal reference is not known</t>
+  </si>
+  <si>
+    <t>An identifier for the other resource. This is used when there is no way to reference the other resource directly, either because the entity is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
+  </si>
+  <si>
+    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
+When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
+Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.</t>
+  </si>
+  <si>
+    <t>Reference.identifier</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.display</t>
+  </si>
+  <si>
+    <t>Text alternative for the resource</t>
+  </si>
+  <si>
+    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
+  </si>
+  <si>
+    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
+  </si>
+  <si>
+    <t>Reference.display</t>
+  </si>
+  <si>
     <t>https://healthterminologies.gov.au/fhir/ValueSet/health-summary-non-clinical-empty-reason-1</t>
   </si>
   <si>
@@ -1366,7 +1426,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-03:This section shall not contain both summary statement of known medicine entries and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').exists() implies           ((Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is MedicationStatement).exists()) xor           (Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation).exists()))}inv-dh-cmp-04:This section shall contain at most one assertion of no relevant finding entry and it shall assert no known current medications {(Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code='101.32009').entry.resolve().where($this is Observation).count() &lt; 2) and            (Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code='101.32009').entry.resolve().where($this is Observation).exists() implies            Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code='101.32009').entry.resolve().value.coding.where($this.system='http://snomed.info/sct' and $this.code='1234391000168107').exists())}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-03:This section shall not contain both summary statement of known medicine entries and assertion of no relevant finding entries {entry.resolve().where($this is MedicationStatement).exists() xor entry.resolve().where($this is Observation ).exists()}inv-dh-cmp-04:This section shall contain at most one assertion of no relevant finding entry and it shall assert no known current medications {entry.resolve().where($this is Observation).exists() implies (entry.resolve().where($this is Observation).count() &lt; 2 and entry.resolve().where($this is value and value.coding.code = '1234391000168107').exists())}</t>
   </si>
   <si>
     <t>Current Medications</t>
@@ -1533,7 +1593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL90"/>
+  <dimension ref="A1:AL100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3896,10 +3956,10 @@
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R22" t="s" s="2">
         <v>186</v>
-      </c>
-      <c r="R22" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>39</v>
@@ -9184,10 +9244,10 @@
       </c>
       <c r="P71" s="2"/>
       <c r="Q71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R71" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="R71" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="S71" t="s" s="2">
         <v>39</v>
@@ -9686,9 +9746,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>404</v>
+        <v>426</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9702,7 +9762,7 @@
         <v>50</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>39</v>
@@ -9711,20 +9771,16 @@
         <v>39</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>405</v>
+        <v>65</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>407</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>408</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>39</v>
       </c>
@@ -9748,11 +9804,13 @@
         <v>39</v>
       </c>
       <c r="W76" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="X76" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="X76" t="s" s="2">
+        <v>39</v>
+      </c>
       <c r="Y76" t="s" s="2">
-        <v>426</v>
+        <v>39</v>
       </c>
       <c r="Z76" t="s" s="2">
         <v>39</v>
@@ -9770,7 +9828,7 @@
         <v>39</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>404</v>
+        <v>67</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>40</v>
@@ -9779,16 +9837,16 @@
         <v>50</v>
       </c>
       <c r="AH76" t="s" s="2">
-        <v>401</v>
+        <v>39</v>
       </c>
       <c r="AI76" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>411</v>
+        <v>68</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>39</v>
@@ -9796,11 +9854,11 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>412</v>
+        <v>427</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" t="s" s="2">
@@ -9819,16 +9877,16 @@
         <v>39</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>413</v>
+        <v>72</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>414</v>
+        <v>73</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>415</v>
+        <v>74</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9866,19 +9924,19 @@
         <v>39</v>
       </c>
       <c r="AA77" t="s" s="2">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="AB77" t="s" s="2">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="AC77" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD77" t="s" s="2">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>412</v>
+        <v>78</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>40</v>
@@ -9887,28 +9945,26 @@
         <v>41</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>379</v>
+        <v>39</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>353</v>
+        <v>68</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>416</v>
+        <v>39</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="B78" t="s" s="2">
-        <v>427</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
         <v>39</v>
       </c>
@@ -9920,24 +9976,26 @@
         <v>50</v>
       </c>
       <c r="G78" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H78" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I78" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H78" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="J78" t="s" s="2">
-        <v>249</v>
+        <v>64</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="M78" s="2"/>
+        <v>430</v>
+      </c>
+      <c r="M78" t="s" s="2">
+        <v>431</v>
+      </c>
       <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
         <v>39</v>
@@ -9986,25 +10044,25 @@
         <v>39</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>347</v>
+        <v>432</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG78" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>39</v>
+        <v>433</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>430</v>
+        <v>39</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>353</v>
+        <v>143</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>354</v>
+        <v>39</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>39</v>
@@ -10012,7 +10070,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>355</v>
+        <v>434</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10032,18 +10090,20 @@
         <v>39</v>
       </c>
       <c r="I79" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>64</v>
+        <v>163</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>65</v>
+        <v>435</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="M79" s="2"/>
+        <v>436</v>
+      </c>
+      <c r="M79" t="s" s="2">
+        <v>437</v>
+      </c>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>39</v>
@@ -10092,7 +10152,7 @@
         <v>39</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>67</v>
+        <v>438</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>40</v>
@@ -10107,7 +10167,7 @@
         <v>39</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>68</v>
+        <v>439</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>39</v>
@@ -10118,7 +10178,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>356</v>
+        <v>440</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10129,7 +10189,7 @@
         <v>40</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>39</v>
@@ -10138,18 +10198,20 @@
         <v>39</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>145</v>
+        <v>441</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="M80" s="2"/>
+        <v>442</v>
+      </c>
+      <c r="M80" t="s" s="2">
+        <v>443</v>
+      </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
         <v>39</v>
@@ -10186,23 +10248,25 @@
         <v>39</v>
       </c>
       <c r="AA80" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB80" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="AB80" t="s" s="2">
+        <v>39</v>
+      </c>
       <c r="AC80" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD80" t="s" s="2">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>78</v>
+        <v>444</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH80" t="s" s="2">
         <v>39</v>
@@ -10211,7 +10275,7 @@
         <v>39</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>39</v>
@@ -10220,13 +10284,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" hidden="true">
+    <row r="81">
       <c r="A81" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="B81" t="s" s="2">
-        <v>357</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
         <v>39</v>
       </c>
@@ -10235,10 +10297,10 @@
         <v>40</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>39</v>
@@ -10247,16 +10309,20 @@
         <v>39</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>358</v>
+        <v>181</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>359</v>
+        <v>405</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="M81" s="2"/>
-      <c r="N81" s="2"/>
+        <v>406</v>
+      </c>
+      <c r="M81" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>408</v>
+      </c>
       <c r="O81" t="s" s="2">
         <v>39</v>
       </c>
@@ -10280,13 +10346,11 @@
         <v>39</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>39</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="X81" s="2"/>
       <c r="Y81" t="s" s="2">
-        <v>39</v>
+        <v>445</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>39</v>
@@ -10304,25 +10368,25 @@
         <v>39</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>78</v>
+        <v>404</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG81" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>152</v>
+        <v>401</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>39</v>
+        <v>411</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>39</v>
@@ -10330,11 +10394,11 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>361</v>
+        <v>412</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>264</v>
+        <v>39</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -10347,22 +10411,22 @@
         <v>39</v>
       </c>
       <c r="H82" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I82" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>159</v>
+        <v>413</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>265</v>
+        <v>414</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>74</v>
+        <v>415</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
@@ -10412,7 +10476,7 @@
         <v>39</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>266</v>
+        <v>412</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>40</v>
@@ -10421,16 +10485,16 @@
         <v>41</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>39</v>
+        <v>379</v>
       </c>
       <c r="AI82" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>143</v>
+        <v>353</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>39</v>
+        <v>416</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>39</v>
@@ -10438,11 +10502,13 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="B83" s="2"/>
+        <v>347</v>
+      </c>
+      <c r="B83" t="s" s="2">
+        <v>446</v>
+      </c>
       <c r="C83" t="s" s="2">
-        <v>363</v>
+        <v>39</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
@@ -10461,26 +10527,22 @@
         <v>39</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>64</v>
+        <v>249</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>367</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
       <c r="O83" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P83" s="2"/>
       <c r="Q83" t="s" s="2">
-        <v>431</v>
+        <v>39</v>
       </c>
       <c r="R83" t="s" s="2">
         <v>39</v>
@@ -10522,33 +10584,33 @@
         <v>39</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>39</v>
+        <v>449</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>239</v>
+        <v>353</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>240</v>
+        <v>354</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10556,13 +10618,13 @@
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F84" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G84" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H84" t="s" s="2">
         <v>39</v>
@@ -10571,26 +10633,22 @@
         <v>39</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>369</v>
+        <v>65</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="N84" t="s" s="2">
-        <v>372</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P84" s="2"/>
       <c r="Q84" t="s" s="2">
-        <v>432</v>
+        <v>39</v>
       </c>
       <c r="R84" t="s" s="2">
         <v>39</v>
@@ -10608,13 +10666,13 @@
         <v>39</v>
       </c>
       <c r="W84" t="s" s="2">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="X84" t="s" s="2">
-        <v>373</v>
+        <v>39</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>374</v>
+        <v>39</v>
       </c>
       <c r="Z84" t="s" s="2">
         <v>39</v>
@@ -10632,7 +10690,7 @@
         <v>39</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>368</v>
+        <v>67</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>40</v>
@@ -10647,18 +10705,18 @@
         <v>39</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>191</v>
+        <v>39</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10666,13 +10724,13 @@
       </c>
       <c r="D85" s="2"/>
       <c r="E85" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G85" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H85" t="s" s="2">
         <v>39</v>
@@ -10681,17 +10739,15 @@
         <v>39</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>376</v>
+        <v>145</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>378</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
         <v>39</v>
@@ -10728,37 +10784,35 @@
         <v>39</v>
       </c>
       <c r="AA85" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB85" t="s" s="2">
-        <v>39</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="AB85" s="2"/>
       <c r="AC85" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD85" t="s" s="2">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>375</v>
+        <v>78</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>379</v>
+        <v>39</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>380</v>
+        <v>39</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>380</v>
+        <v>39</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>39</v>
@@ -10766,9 +10820,11 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="B86" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="B86" t="s" s="2">
+        <v>357</v>
+      </c>
       <c r="C86" t="s" s="2">
         <v>39</v>
       </c>
@@ -10777,38 +10833,34 @@
         <v>40</v>
       </c>
       <c r="F86" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G86" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H86" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I86" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>119</v>
+        <v>358</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="M86" t="s" s="2">
-        <v>384</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>385</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
       <c r="O86" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P86" s="2"/>
       <c r="Q86" t="s" s="2">
-        <v>423</v>
+        <v>39</v>
       </c>
       <c r="R86" t="s" s="2">
         <v>39</v>
@@ -10826,13 +10878,13 @@
         <v>39</v>
       </c>
       <c r="W86" t="s" s="2">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>386</v>
+        <v>39</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>387</v>
+        <v>39</v>
       </c>
       <c r="Z86" t="s" s="2">
         <v>39</v>
@@ -10850,69 +10902,67 @@
         <v>39</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>381</v>
+        <v>78</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG86" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH86" t="s" s="2">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>388</v>
+        <v>39</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>192</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>389</v>
+        <v>361</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
-        <v>39</v>
+        <v>264</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F87" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G87" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H87" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="I87" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>181</v>
+        <v>71</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>390</v>
+        <v>159</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>391</v>
+        <v>265</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="N87" t="s" s="2">
-        <v>393</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="N87" s="2"/>
       <c r="O87" t="s" s="2">
         <v>39</v>
       </c>
@@ -10936,13 +10986,13 @@
         <v>39</v>
       </c>
       <c r="W87" t="s" s="2">
-        <v>187</v>
+        <v>39</v>
       </c>
       <c r="X87" t="s" s="2">
-        <v>394</v>
+        <v>39</v>
       </c>
       <c r="Y87" t="s" s="2">
-        <v>395</v>
+        <v>39</v>
       </c>
       <c r="Z87" t="s" s="2">
         <v>39</v>
@@ -10960,13 +11010,13 @@
         <v>39</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>389</v>
+        <v>266</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG87" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH87" t="s" s="2">
         <v>39</v>
@@ -10975,10 +11025,10 @@
         <v>39</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>396</v>
+        <v>143</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="AL87" t="s" s="2">
         <v>39</v>
@@ -10986,18 +11036,18 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>397</v>
+        <v>362</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
-        <v>39</v>
+        <v>363</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F88" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G88" t="s" s="2">
         <v>51</v>
@@ -11009,24 +11059,26 @@
         <v>39</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>433</v>
+        <v>64</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>434</v>
+        <v>364</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>399</v>
+        <v>365</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="N88" s="2"/>
+        <v>366</v>
+      </c>
+      <c r="N88" t="s" s="2">
+        <v>367</v>
+      </c>
       <c r="O88" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P88" s="2"/>
       <c r="Q88" t="s" s="2">
-        <v>39</v>
+        <v>450</v>
       </c>
       <c r="R88" t="s" s="2">
         <v>39</v>
@@ -11068,25 +11120,25 @@
         <v>39</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>397</v>
+        <v>362</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG88" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH88" t="s" s="2">
-        <v>401</v>
+        <v>39</v>
       </c>
       <c r="AI88" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>402</v>
+        <v>239</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>403</v>
+        <v>240</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>39</v>
@@ -11094,7 +11146,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>404</v>
+        <v>368</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11102,7 +11154,7 @@
       </c>
       <c r="D89" s="2"/>
       <c r="E89" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F89" t="s" s="2">
         <v>50</v>
@@ -11120,16 +11172,16 @@
         <v>181</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>405</v>
+        <v>369</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>406</v>
+        <v>370</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>407</v>
+        <v>371</v>
       </c>
       <c r="N89" t="s" s="2">
-        <v>408</v>
+        <v>372</v>
       </c>
       <c r="O89" t="s" s="2">
         <v>39</v>
@@ -11139,7 +11191,7 @@
         <v>39</v>
       </c>
       <c r="R89" t="s" s="2">
-        <v>39</v>
+        <v>451</v>
       </c>
       <c r="S89" t="s" s="2">
         <v>39</v>
@@ -11154,11 +11206,13 @@
         <v>39</v>
       </c>
       <c r="W89" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="X89" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="Y89" t="s" s="2">
-        <v>426</v>
+        <v>374</v>
       </c>
       <c r="Z89" t="s" s="2">
         <v>39</v>
@@ -11176,7 +11230,7 @@
         <v>39</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>404</v>
+        <v>368</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>40</v>
@@ -11185,24 +11239,24 @@
         <v>50</v>
       </c>
       <c r="AH89" t="s" s="2">
-        <v>401</v>
+        <v>39</v>
       </c>
       <c r="AI89" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>411</v>
+        <v>190</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="90" hidden="true">
+    <row r="90">
       <c r="A90" t="s" s="2">
-        <v>412</v>
+        <v>375</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11210,13 +11264,13 @@
       </c>
       <c r="D90" s="2"/>
       <c r="E90" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F90" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G90" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H90" t="s" s="2">
         <v>39</v>
@@ -11225,16 +11279,16 @@
         <v>39</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>413</v>
+        <v>376</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>414</v>
+        <v>377</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>415</v>
+        <v>378</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" t="s" s="2">
@@ -11284,13 +11338,13 @@
         <v>39</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>412</v>
+        <v>375</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG90" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH90" t="s" s="2">
         <v>379</v>
@@ -11299,17 +11353,1099 @@
         <v>39</v>
       </c>
       <c r="AJ90" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" hidden="true">
+      <c r="A91" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F91" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="O91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P91" s="2"/>
+      <c r="Q91" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="R91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" hidden="true">
+      <c r="A92" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F92" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="M92" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="N92" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="O92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M93" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="N93" s="2"/>
+      <c r="O93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F94" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P94" s="2"/>
+      <c r="Q94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ94" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F95" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="N95" s="2"/>
+      <c r="O95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P95" s="2"/>
+      <c r="Q95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="F96" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="N96" s="2"/>
+      <c r="O96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P96" s="2"/>
+      <c r="Q96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" hidden="true">
+      <c r="A97" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F97" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="M97" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="N97" s="2"/>
+      <c r="O97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P97" s="2"/>
+      <c r="Q97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL97" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" hidden="true">
+      <c r="A98" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F98" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I98" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J98" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="L98" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="M98" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="N98" s="2"/>
+      <c r="O98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P98" s="2"/>
+      <c r="Q98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL98" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F99" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G99" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="H99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J99" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K99" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L99" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="M99" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="N99" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="O99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P99" s="2"/>
+      <c r="Q99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W99" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="X99" s="2"/>
+      <c r="Y99" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="Z99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE99" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AF99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG99" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH99" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="AI99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ99" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="AK99" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AL99" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" hidden="true">
+      <c r="A100" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F100" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K100" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="L100" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="M100" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="N100" s="2"/>
+      <c r="O100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P100" s="2"/>
+      <c r="Q100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE100" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="AF100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG100" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH100" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AI100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ100" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="AK90" t="s" s="2">
+      <c r="AK100" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="AL90" t="s" s="2">
+      <c r="AL100" t="s" s="2">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL90">
+  <autoFilter ref="A1:AL100">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11319,7 +12455,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI89">
+  <conditionalFormatting sqref="A2:AI99">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>